<commit_message>
Bulk henter referansenummere, skriver til excelfilen og returnerner
</commit_message>
<xml_diff>
--- a/src/test/resources/koronasykepengerefusjon_nav_TESTFILE.xlsx
+++ b/src/test/resources/koronasykepengerefusjon_nav_TESTFILE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tuxbear/dev/src/sporenstreks/src/main/resources/bulk-upload/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tuxbear/dev/src/sporenstreks/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E37F7D-A87B-6B44-ADF5-7B64A3A732D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA58E15C-74C2-CA41-BFB4-9CB146536083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{D6DC71BC-B5E6-104F-ACAE-6ED12C21E25B}"/>
+    <workbookView xWindow="7920" yWindow="7540" windowWidth="33600" windowHeight="20540" xr2:uid="{D6DC71BC-B5E6-104F-ACAE-6ED12C21E25B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3310F717-4C48-AB4E-8AB9-49D048916BC7}">
   <dimension ref="A1:H2875"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F2875"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>